<commit_message>
Added EV penetration scenarios
</commit_message>
<xml_diff>
--- a/data/raw_data/EV_scenarios.xlsx
+++ b/data/raw_data/EV_scenarios.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fernaag/Box/BATMAN/Coding/V2G_in_EU/data/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FFFE22F7-47DB-1C40-9E7B-63CCAEAC73E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81EB1074-0514-2240-912B-1F74B0C0416D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28820" yWindow="500" windowWidth="39980" windowHeight="28300" xr2:uid="{D42F6FC8-8893-9742-924A-9E6CE237EBE9}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{D42F6FC8-8893-9742-924A-9E6CE237EBE9}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Penetration in stock" sheetId="1" r:id="rId1"/>
+    <sheet name="Penetration in sales" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="23">
   <si>
     <t>Scenario</t>
   </si>
@@ -82,6 +83,27 @@
   </si>
   <si>
     <t>EV penetration in stock. Calculated from mass balance</t>
+  </si>
+  <si>
+    <t>Page 18 IEA global EV outlook</t>
+  </si>
+  <si>
+    <t>STEP</t>
+  </si>
+  <si>
+    <t>IEA 2021 EV outlook</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>Numbers for LDVs</t>
+  </si>
+  <si>
+    <t>Assumption</t>
+  </si>
+  <si>
+    <t>From mass balance</t>
   </si>
 </sst>
 </file>
@@ -454,8 +476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52754300-F177-F14B-8497-9FBF141385D0}">
   <dimension ref="A1:H75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M42" sqref="M42"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H57" sqref="H57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1344,4 +1366,512 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B65BFFD4-3A3C-0049-B7C9-CFDE4D87F3F2}">
+  <dimension ref="A1:F25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>2015</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2020</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.06</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2015</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2020</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="F5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>2015</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="F6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>2020</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.06</v>
+      </c>
+      <c r="F7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>2015</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="F8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>2020</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="F9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>2030</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0.22</v>
+      </c>
+      <c r="F10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>2030</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="F11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>2030</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0.17</v>
+      </c>
+      <c r="F12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>2030</v>
+      </c>
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0.23</v>
+      </c>
+      <c r="F13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>2050</v>
+      </c>
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1</v>
+      </c>
+      <c r="F14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>2050</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="1">
+        <v>1</v>
+      </c>
+      <c r="F15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>2050</v>
+      </c>
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0</v>
+      </c>
+      <c r="F16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>2050</v>
+      </c>
+      <c r="B17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0</v>
+      </c>
+      <c r="F17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>2015</v>
+      </c>
+      <c r="B18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="1">
+        <f>1-E2-E4%</f>
+        <v>0.9899</v>
+      </c>
+      <c r="F18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>2020</v>
+      </c>
+      <c r="B19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" s="1">
+        <f>1-E3-E5</f>
+        <v>0.8899999999999999</v>
+      </c>
+      <c r="F19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>2015</v>
+      </c>
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" s="1">
+        <f>1-E4-E6%</f>
+        <v>0.9899</v>
+      </c>
+      <c r="F20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>2020</v>
+      </c>
+      <c r="B21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" s="1">
+        <f>1-E5-E7</f>
+        <v>0.8899999999999999</v>
+      </c>
+      <c r="F21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>2030</v>
+      </c>
+      <c r="B22" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" s="1">
+        <f>1-E11-E13</f>
+        <v>0.21999999999999995</v>
+      </c>
+      <c r="F22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>2030</v>
+      </c>
+      <c r="B23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" s="1">
+        <f>1-E12-E10</f>
+        <v>0.61</v>
+      </c>
+      <c r="F23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>2040</v>
+      </c>
+      <c r="B24" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24" s="1">
+        <f>1-E17-E15</f>
+        <v>0</v>
+      </c>
+      <c r="F24" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>2045</v>
+      </c>
+      <c r="B25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" s="1">
+        <v>0</v>
+      </c>
+      <c r="F25" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update EV_scenarios.xlsx, V2G_scenarios.xlsx, V2G_ratio.ipynb, EV_penetration_scenarios.ipynb
</commit_message>
<xml_diff>
--- a/data/raw_data/EV_scenarios.xlsx
+++ b/data/raw_data/EV_scenarios.xlsx
@@ -1,41 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fernaag/Box/BATMAN/Coding/V2G_in_EU/data/raw_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lauinger\Desktop\dirk\Second-Life Batteries\code_git\V2G_in_EU\data\raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81EB1074-0514-2240-912B-1F74B0C0416D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{D42F6FC8-8893-9742-924A-9E6CE237EBE9}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="17505" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Penetration in stock" sheetId="1" r:id="rId1"/>
     <sheet name="Penetration in sales" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Penetration in sales'!$A$1:$F$33</definedName>
+  </definedNames>
+  <calcPr calcId="162913" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="27">
   <si>
     <t>Scenario</t>
   </si>
@@ -104,12 +92,27 @@
   </si>
   <si>
     <t>From mass balance</t>
+  </si>
+  <si>
+    <t>FCEV</t>
+  </si>
+  <si>
+    <t>Clean Planet for All &amp; ENTSOE (GA)</t>
+  </si>
+  <si>
+    <t>Clean Planet for All &amp; ENTSOE (DE)</t>
+  </si>
+  <si>
+    <t>TYNDP22 draft</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000%"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -154,15 +157,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -473,16 +477,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52754300-F177-F14B-8497-9FBF141385D0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H57" sqref="H57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -502,7 +506,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2015</v>
       </c>
@@ -522,7 +526,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2030</v>
       </c>
@@ -542,7 +546,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2050</v>
       </c>
@@ -562,7 +566,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2015</v>
       </c>
@@ -582,7 +586,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2030</v>
       </c>
@@ -602,7 +606,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2050</v>
       </c>
@@ -622,7 +626,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2015</v>
       </c>
@@ -642,7 +646,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2030</v>
       </c>
@@ -662,7 +666,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2050</v>
       </c>
@@ -682,7 +686,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2015</v>
       </c>
@@ -702,7 +706,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2030</v>
       </c>
@@ -722,7 +726,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2050</v>
       </c>
@@ -742,7 +746,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2015</v>
       </c>
@@ -762,7 +766,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2030</v>
       </c>
@@ -782,7 +786,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2050</v>
       </c>
@@ -802,7 +806,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2015</v>
       </c>
@@ -822,7 +826,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2030</v>
       </c>
@@ -842,7 +846,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2050</v>
       </c>
@@ -862,7 +866,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2015</v>
       </c>
@@ -882,7 +886,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2030</v>
       </c>
@@ -902,7 +906,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2050</v>
       </c>
@@ -922,7 +926,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2015</v>
       </c>
@@ -942,7 +946,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2030</v>
       </c>
@@ -962,7 +966,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2050</v>
       </c>
@@ -982,7 +986,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2015</v>
       </c>
@@ -1002,7 +1006,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2030</v>
       </c>
@@ -1022,7 +1026,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2050</v>
       </c>
@@ -1042,7 +1046,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>2015</v>
       </c>
@@ -1065,7 +1069,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>2030</v>
       </c>
@@ -1088,7 +1092,7 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>2050</v>
       </c>
@@ -1111,7 +1115,7 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>2015</v>
       </c>
@@ -1134,7 +1138,7 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>2030</v>
       </c>
@@ -1157,7 +1161,7 @@
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>2050</v>
       </c>
@@ -1180,7 +1184,7 @@
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>2015</v>
       </c>
@@ -1203,7 +1207,7 @@
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>2030</v>
       </c>
@@ -1226,7 +1230,7 @@
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>2050</v>
       </c>
@@ -1249,118 +1253,118 @@
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E38" s="1"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E39" s="1"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E40" s="1"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E41" s="1"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E42" s="1"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E43" s="1"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E44" s="1"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E45" s="1"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E46" s="1"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E47" s="1"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E48" s="1"/>
     </row>
-    <row r="49" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E49" s="1"/>
     </row>
-    <row r="50" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E50" s="1"/>
     </row>
-    <row r="51" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E51" s="1"/>
     </row>
-    <row r="52" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E52" s="1"/>
     </row>
-    <row r="53" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E53" s="1"/>
     </row>
-    <row r="54" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E54" s="1"/>
     </row>
-    <row r="55" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E55" s="1"/>
     </row>
-    <row r="56" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E56" s="1"/>
     </row>
-    <row r="57" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E57" s="1"/>
     </row>
-    <row r="58" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E58" s="1"/>
     </row>
-    <row r="59" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E59" s="1"/>
     </row>
-    <row r="60" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E60" s="1"/>
     </row>
-    <row r="61" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E61" s="1"/>
     </row>
-    <row r="62" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E62" s="1"/>
     </row>
-    <row r="63" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="63" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E63" s="1"/>
     </row>
-    <row r="64" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="64" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E64" s="1"/>
     </row>
-    <row r="65" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E65" s="1"/>
     </row>
-    <row r="66" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="66" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E66" s="1"/>
     </row>
-    <row r="67" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="67" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E67" s="1"/>
     </row>
-    <row r="68" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="68" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E68" s="1"/>
     </row>
-    <row r="69" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E69" s="1"/>
     </row>
-    <row r="70" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="70" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E70" s="1"/>
     </row>
-    <row r="71" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="71" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E71" s="1"/>
     </row>
-    <row r="72" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="72" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E72" s="1"/>
     </row>
-    <row r="73" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="73" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E73" s="1"/>
     </row>
-    <row r="74" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="74" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E74" s="1"/>
     </row>
-    <row r="75" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="75" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E75" s="1"/>
     </row>
   </sheetData>
@@ -1369,20 +1373,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B65BFFD4-3A3C-0049-B7C9-CFDE4D87F3F2}">
-  <dimension ref="A1:F25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="1"/>
+    <col min="4" max="4" width="17.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1402,7 +1406,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2015</v>
       </c>
@@ -1422,7 +1426,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2020</v>
       </c>
@@ -1442,7 +1446,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2015</v>
       </c>
@@ -1462,7 +1466,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2020</v>
       </c>
@@ -1482,7 +1486,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2015</v>
       </c>
@@ -1502,7 +1506,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2020</v>
       </c>
@@ -1522,7 +1526,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2015</v>
       </c>
@@ -1542,7 +1546,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2020</v>
       </c>
@@ -1562,7 +1566,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2030</v>
       </c>
@@ -1582,7 +1586,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2030</v>
       </c>
@@ -1602,32 +1606,29 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>2030</v>
+        <v>2045</v>
       </c>
       <c r="B12" t="s">
         <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="E12" s="1">
-        <v>0.17</v>
+        <v>0.88</v>
       </c>
       <c r="F12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2030</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C13" t="s">
         <v>12</v>
@@ -1636,38 +1637,38 @@
         <v>18</v>
       </c>
       <c r="E13" s="1">
-        <v>0.23</v>
+        <v>0.17</v>
       </c>
       <c r="F13" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>2050</v>
+        <v>2030</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C14" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D14" t="s">
         <v>18</v>
       </c>
       <c r="E14" s="1">
-        <v>1</v>
+        <v>0.23</v>
       </c>
       <c r="F14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2050</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C15" t="s">
         <v>5</v>
@@ -1676,38 +1677,38 @@
         <v>18</v>
       </c>
       <c r="E15" s="1">
-        <v>1</v>
+        <v>0.89</v>
       </c>
       <c r="F15" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2050</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C16" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D16" t="s">
         <v>18</v>
       </c>
       <c r="E16" s="1">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="F16" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2050</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C17" t="s">
         <v>12</v>
@@ -1722,30 +1723,29 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>2015</v>
+        <v>2050</v>
       </c>
       <c r="B18" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C18" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D18" t="s">
         <v>18</v>
       </c>
       <c r="E18" s="1">
-        <f>1-E2-E4%</f>
-        <v>0.9899</v>
+        <v>0</v>
       </c>
       <c r="F18" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>2020</v>
+        <v>2015</v>
       </c>
       <c r="B19" t="s">
         <v>17</v>
@@ -1756,35 +1756,38 @@
       <c r="D19" t="s">
         <v>18</v>
       </c>
-      <c r="E19" s="1">
-        <f>1-E3-E5</f>
-        <v>0.8899999999999999</v>
+      <c r="E19" s="4">
+        <f>1-E2-E4</f>
+        <v>0.98</v>
       </c>
       <c r="F19" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>2015</v>
+        <v>2020</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C20" t="s">
         <v>14</v>
       </c>
+      <c r="D20" t="s">
+        <v>18</v>
+      </c>
       <c r="E20" s="1">
-        <f>1-E4-E6%</f>
-        <v>0.9899</v>
+        <f>1-E3-E5-E31</f>
+        <v>0.8899999999999999</v>
       </c>
       <c r="F20" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>2020</v>
+        <v>2015</v>
       </c>
       <c r="B21" t="s">
         <v>19</v>
@@ -1792,17 +1795,17 @@
       <c r="C21" t="s">
         <v>14</v>
       </c>
-      <c r="E21" s="1">
-        <f>1-E5-E7</f>
-        <v>0.8899999999999999</v>
+      <c r="E21" s="4">
+        <f>1-E6-E8</f>
+        <v>0.98</v>
       </c>
       <c r="F21" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>2030</v>
+        <v>2020</v>
       </c>
       <c r="B22" t="s">
         <v>19</v>
@@ -1811,55 +1814,55 @@
         <v>14</v>
       </c>
       <c r="E22" s="1">
-        <f>1-E11-E13</f>
-        <v>0.21999999999999995</v>
+        <f>1-E7-E9-E31</f>
+        <v>0.8899999999999999</v>
       </c>
       <c r="F22" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2030</v>
       </c>
       <c r="B23" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C23" t="s">
         <v>14</v>
       </c>
       <c r="E23" s="1">
-        <f>1-E12-E10</f>
-        <v>0.61</v>
+        <f>1-E11-E14-E28</f>
+        <v>0.19999999999999996</v>
       </c>
       <c r="F23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>2040</v>
+        <v>2030</v>
       </c>
       <c r="B24" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C24" t="s">
         <v>14</v>
       </c>
       <c r="E24" s="1">
-        <f>1-E17-E15</f>
-        <v>0</v>
+        <f>1-E13-E10-E32</f>
+        <v>0.6</v>
       </c>
       <c r="F24" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>2045</v>
+        <v>2040</v>
       </c>
       <c r="B25" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C25" t="s">
         <v>14</v>
@@ -1871,7 +1874,162 @@
         <v>21</v>
       </c>
     </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>2045</v>
+      </c>
+      <c r="B26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" t="s">
+        <v>14</v>
+      </c>
+      <c r="E26" s="1">
+        <v>0</v>
+      </c>
+      <c r="F26" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>2020</v>
+      </c>
+      <c r="B27" t="s">
+        <v>19</v>
+      </c>
+      <c r="C27" t="s">
+        <v>23</v>
+      </c>
+      <c r="D27" t="s">
+        <v>24</v>
+      </c>
+      <c r="E27" s="1">
+        <v>0</v>
+      </c>
+      <c r="F27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>2030</v>
+      </c>
+      <c r="B28" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28" t="s">
+        <v>23</v>
+      </c>
+      <c r="D28" t="s">
+        <v>24</v>
+      </c>
+      <c r="E28" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="F28" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>2040</v>
+      </c>
+      <c r="B29" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29" t="s">
+        <v>23</v>
+      </c>
+      <c r="E29" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="F29" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>2050</v>
+      </c>
+      <c r="B30" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30" t="s">
+        <v>23</v>
+      </c>
+      <c r="D30" t="s">
+        <v>24</v>
+      </c>
+      <c r="E30" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="F30" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>2020</v>
+      </c>
+      <c r="B31" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31" t="s">
+        <v>23</v>
+      </c>
+      <c r="D31" t="s">
+        <v>25</v>
+      </c>
+      <c r="E31" s="1">
+        <v>0</v>
+      </c>
+      <c r="F31" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>2030</v>
+      </c>
+      <c r="B32" t="s">
+        <v>17</v>
+      </c>
+      <c r="C32" t="s">
+        <v>23</v>
+      </c>
+      <c r="D32" t="s">
+        <v>25</v>
+      </c>
+      <c r="E32" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="F32" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>2050</v>
+      </c>
+      <c r="B33" t="s">
+        <v>17</v>
+      </c>
+      <c r="C33" t="s">
+        <v>23</v>
+      </c>
+      <c r="D33" t="s">
+        <v>25</v>
+      </c>
+      <c r="E33" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="F33" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:F33"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>